<commit_message>
PROS-11454 CCJP KPI development Red Score
</commit_message>
<xml_diff>
--- a/Projects/CCJP/Data/template.xlsx
+++ b/Projects/CCJP/Data/template.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="poc_config" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="kpi" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">poc_config!$B$1:$N$75</definedName>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="68">
   <si>
     <t xml:space="preserve">store_policy</t>
   </si>
@@ -221,6 +222,21 @@
   </si>
   <si>
     <t xml:space="preserve">Event Space, Checkout</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kpi_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sovi_weightage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">poc_weightage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dist_weightage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CCJP_RED_SCORE</t>
   </si>
 </sst>
 </file>
@@ -269,18 +285,26 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="8"/>
-      <color rgb="FF000000"/>
+      <b val="true"/>
+      <sz val="12"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000099"/>
+        <bgColor rgb="FF000080"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -341,7 +365,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -354,6 +378,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000099"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -364,30 +448,30 @@
   </sheetPr>
   <dimension ref="A1:Q19"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C24" activeCellId="0" sqref="C24"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G18" activeCellId="0" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="8.12145748987854"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="31.8785425101215"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.6396761133603"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="33.3765182186235"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="4.61133603238866"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="13.834008097166"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="12.1336032388664"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="13.834008097166"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="12.1336032388664"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="12.2348178137652"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="12.1336032388664"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="12.2348178137652"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="12.1336032388664"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="12.2348178137652"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="12.1336032388664"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="12.2348178137652"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="12.1336032388664"/>
-    <col collapsed="false" hidden="false" max="1025" min="18" style="1" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="8.1417004048583"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="32.3481781376518"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.9230769230769"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="33.9554655870445"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="4.39271255060729"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="13.8178137651822"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="12.3198380566802"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="13.8178137651822"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="12.3198380566802"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="12.4251012145749"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="12.3198380566802"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="12.4251012145749"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="12.3198380566802"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="12.4251012145749"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="12.3198380566802"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="12.4251012145749"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="12.3198380566802"/>
+    <col collapsed="false" hidden="false" max="1025" min="18" style="1" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -459,7 +543,7 @@
       <c r="E2" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="3" t="s">
         <v>21</v>
       </c>
       <c r="G2" s="3" t="s">
@@ -500,7 +584,7 @@
       <c r="E3" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="3" t="s">
         <v>21</v>
       </c>
       <c r="G3" s="3" t="s">
@@ -541,7 +625,7 @@
       <c r="E4" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="3" t="s">
         <v>21</v>
       </c>
       <c r="G4" s="3" t="s">
@@ -582,7 +666,7 @@
       <c r="E5" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="3" t="s">
         <v>21</v>
       </c>
       <c r="G5" s="3" t="s">
@@ -623,7 +707,7 @@
       <c r="E6" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="3" t="s">
         <v>21</v>
       </c>
       <c r="G6" s="3" t="s">
@@ -664,7 +748,7 @@
       <c r="E7" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="3" t="s">
         <v>21</v>
       </c>
       <c r="G7" s="3" t="s">
@@ -705,7 +789,7 @@
       <c r="E8" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="3" t="s">
         <v>21</v>
       </c>
       <c r="G8" s="3" t="s">
@@ -746,7 +830,7 @@
       <c r="E9" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F9" s="3" t="s">
         <v>21</v>
       </c>
       <c r="G9" s="3" t="s">
@@ -787,7 +871,7 @@
       <c r="E10" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="F10" s="3" t="s">
         <v>21</v>
       </c>
       <c r="G10" s="3" t="s">
@@ -830,4 +914,63 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.6032388663968"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.3684210526316"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="14.0323886639676"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="13.9271255060729"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="1" width="9.1417004048583"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" s="1" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C2" s="1" t="n">
+        <v>0.42</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>0.42</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
PROS-11454-CCJP KPI Dev Unique Distribution
</commit_message>
<xml_diff>
--- a/Projects/CCJP/Data/template.xlsx
+++ b/Projects/CCJP/Data/template.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="73">
   <si>
     <t xml:space="preserve">store_policy</t>
   </si>
@@ -236,7 +236,22 @@
     <t xml:space="preserve">dist_weightage</t>
   </si>
   <si>
+    <t xml:space="preserve">Include Empty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Include Irrelevant</t>
+  </si>
+  <si>
     <t xml:space="preserve">CCJP_RED_SCORE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N/A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CCJP_UNIQUE_DIST_OWN_MANU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N</t>
   </si>
 </sst>
 </file>
@@ -286,7 +301,7 @@
     </font>
     <font>
       <b val="true"/>
-      <sz val="12"/>
+      <sz val="8"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -365,7 +380,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -449,28 +464,28 @@
   <dimension ref="A1:Q19"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G18" activeCellId="0" sqref="G18"/>
+      <selection pane="topLeft" activeCell="D32" activeCellId="0" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="8.1417004048583"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="32.3481781376518"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.9230769230769"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="33.9554655870445"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="32.5627530364372"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.0323886639676"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="34.2793522267206"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="1" width="4.39271255060729"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="1" width="13.8178137651822"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="12.3198380566802"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="12.4251012145749"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="1" width="13.8178137651822"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="12.3198380566802"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="12.4251012145749"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="12.3198380566802"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="12.4251012145749"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="12.3198380566802"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="12.4251012145749"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="12.3198380566802"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="12.4251012145749"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="12.3198380566802"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="12.4251012145749"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="12.5344129554656"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="12.4251012145749"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="12.5344129554656"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="12.4251012145749"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="12.5344129554656"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="12.4251012145749"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="12.5344129554656"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="12.4251012145749"/>
     <col collapsed="false" hidden="false" max="1025" min="18" style="1" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -921,22 +936,35 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:R3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+      <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.6032388663968"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.3684210526316"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="14.0323886639676"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="13.9271255060729"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="1" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="21.0890688259109"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="10.3967611336032"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="1" width="10.1781376518219"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="9.84615384615385"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="11.6113360323887"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="12.0485829959514"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="11.9392712550607"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="12.0485829959514"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="11.9392712550607"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="12.0485829959514"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="11.9392712550607"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="12.0485829959514"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="11.9392712550607"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="12.0485829959514"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="11.9392712550607"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="12.0485829959514"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="11.9392712550607"/>
+    <col collapsed="false" hidden="false" max="1025" min="19" style="1" width="9.1417004048583"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
         <v>63</v>
       </c>
@@ -949,20 +977,120 @@
       <c r="D1" s="4" t="s">
         <v>66</v>
       </c>
+      <c r="E1" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B2" s="1" t="n">
+      <c r="A2" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2" s="3" t="n">
         <v>0.16</v>
       </c>
-      <c r="C2" s="1" t="n">
+      <c r="C2" s="3" t="n">
         <v>0.42</v>
       </c>
-      <c r="D2" s="1" t="n">
+      <c r="D2" s="3" t="n">
         <v>0.42</v>
       </c>
+      <c r="E2" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
PROS-11454-CCJP POC KPI change
</commit_message>
<xml_diff>
--- a/Projects/CCJP/Data/template.xlsx
+++ b/Projects/CCJP/Data/template.xlsx
@@ -91,7 +91,7 @@
     <t xml:space="preserve">Priority_POC_SM_L, Other_POC_SM_L, Priority_POC,Other_POC</t>
   </si>
   <si>
-    <t xml:space="preserve">Priority_POC_SM_L, Priority_POC,Other_POC</t>
+    <t xml:space="preserve">Priority_POC_SM_L, Priority_POC</t>
   </si>
   <si>
     <t xml:space="preserve">Event Space, Checkout, Beverage end, Deli section, Liquor, 0003-Event space, 0004-Checkout,0005-End, 0006-Deli,0007-Liquor</t>
@@ -121,7 +121,7 @@
     <t xml:space="preserve">Priority_POC_SM_M, Other_POC_SM_M, Priority_POC,Other_POC</t>
   </si>
   <si>
-    <t xml:space="preserve">Priority_POC_SM_M, Priority_POC,Other_POC</t>
+    <t xml:space="preserve">Priority_POC_SM_M, Priority_POC</t>
   </si>
   <si>
     <t xml:space="preserve">Event Space, Checkout, Deli section, Liquor, 0003-Event space,0004-Checkout,0006-Deli,0007-Liquor</t>
@@ -136,7 +136,7 @@
     <t xml:space="preserve">Priority_POC_SM_S, Other_POC_SM_S, Priority_POC,Other_POC</t>
   </si>
   <si>
-    <t xml:space="preserve">Priority_POC_SM_S, Priority_POC,Other_POC</t>
+    <t xml:space="preserve">Priority_POC_SM_S, Priority_POC</t>
   </si>
   <si>
     <t xml:space="preserve">Event Space, Checkout, Deli section, 0003-Event space,0004-Checkout,0006-Deli</t>
@@ -151,7 +151,7 @@
     <t xml:space="preserve">Priority_POC_Drug_L, Other_POC_Drug_L, Priority_POC,Other_POC</t>
   </si>
   <si>
-    <t xml:space="preserve">Priority_POC_Drug_L, Priority_POC,Other_POC</t>
+    <t xml:space="preserve">Priority_POC_Drug_L, Priority_POC</t>
   </si>
   <si>
     <t xml:space="preserve">Event Space, Checkout, Beverage end, Deli section, 0003-Event space,0004-Checkout,0005-End,0006-Deli</t>
@@ -166,7 +166,7 @@
     <t xml:space="preserve">Priority_POC_Drug_M, Other_POC_Drug_M, Priority_POC,Other_POC</t>
   </si>
   <si>
-    <t xml:space="preserve">Priority_POC_Drug_M, Priority_POC,Other_POC</t>
+    <t xml:space="preserve">Priority_POC_Drug_M, Priority_POC</t>
   </si>
   <si>
     <t xml:space="preserve">Event Space, Checkout, Store front, 0003-Event space,0004-Checkout, 0009-Store Front</t>
@@ -178,7 +178,7 @@
     <t xml:space="preserve">Priority_POC_Drug_S, Other_POC_Drug_S, Priority_POC,Other_POC</t>
   </si>
   <si>
-    <t xml:space="preserve">Priority_POC_Drug_S, Priority_POC,Other_POC</t>
+    <t xml:space="preserve">Priority_POC_Drug_S, Priority_POC</t>
   </si>
   <si>
     <t xml:space="preserve">Checkout, Store front,0004-Checkout, 0009-Store Front</t>
@@ -190,7 +190,7 @@
     <t xml:space="preserve">Priority_POC_Discounter_L, Other_POC_Discounter_L, Priority_POC,Other_POC</t>
   </si>
   <si>
-    <t xml:space="preserve">Priority_POC_Discounter_L, Priority_POC,Other_POC</t>
+    <t xml:space="preserve">Priority_POC_Discounter_L, Priority_POC</t>
   </si>
   <si>
     <t xml:space="preserve">Event Space, Checkout, Beverage end, Liquor,0003-Event space,0004-Checkout,0005-End,0007-Liquor</t>
@@ -205,7 +205,7 @@
     <t xml:space="preserve">Priority_POC_Discounter_M, Other_POC_Discounter_M, Priority_POC,Other_POC</t>
   </si>
   <si>
-    <t xml:space="preserve">Priority_POC_Discounter_M, Priority_POC,Other_POC</t>
+    <t xml:space="preserve">Priority_POC_Discounter_M, Priority_POC</t>
   </si>
   <si>
     <t xml:space="preserve">Event Space, Checkout, Beverage end,0003-Event space,0004-Checkout,0005-End</t>
@@ -217,7 +217,7 @@
     <t xml:space="preserve">Priority_POC_Discounter_S, Other_POC_Discounter_S, Priority_POC,Other_POC</t>
   </si>
   <si>
-    <t xml:space="preserve">Priority_POC_Discounter_S, Priority_POC,Other_POC</t>
+    <t xml:space="preserve">Priority_POC_Discounter_S, Priority_POC</t>
   </si>
   <si>
     <t xml:space="preserve">Event Space, Checkout,0003-Event space,0004-Checkout</t>
@@ -318,12 +318,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -352,465 +356,456 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q19"/>
+  <dimension ref="A1:Q10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D25" activeCellId="0" sqref="D25"/>
+      <selection pane="topLeft" activeCell="B23" activeCellId="0" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="8.1417004048583"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="45.8461538461538"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="49.8097165991903"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="93.2995951417004"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="4.39271255060729"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="13.8178137651822"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="13.0688259109312"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="13.8178137651822"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="13.0688259109312"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="13.1740890688259"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="13.0688259109312"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="13.1740890688259"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="13.0688259109312"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="13.1740890688259"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="13.0688259109312"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="13.1740890688259"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="13.0688259109312"/>
-    <col collapsed="false" hidden="false" max="1025" min="18" style="1" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="8.31983805668016"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="46.2105263157895"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="24.3603238866397"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="71.668016194332"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="4.61133603238866"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="13.834008097166"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="12.1336032388664"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="13.834008097166"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="12.1336032388664"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="12.2348178137652"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="12.1336032388664"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="12.2348178137652"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="12.1336032388664"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="12.2348178137652"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="12.1336032388664"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="12.2348178137652"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="12.1336032388664"/>
+    <col collapsed="false" hidden="false" max="1025" min="18" style="1" width="9.1417004048583"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="O1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="P1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="Q1" s="3" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="3" t="n">
+      <c r="E2" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="K2" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="3"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="4"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="3" t="n">
+      <c r="E3" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="J3" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="K3" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
-      <c r="O3" s="3"/>
-      <c r="P3" s="3"/>
-      <c r="Q3" s="3"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="4"/>
+      <c r="P3" s="4"/>
+      <c r="Q3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="3" t="n">
+      <c r="E4" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="I4" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="J4" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="K4" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
-      <c r="O4" s="3"/>
-      <c r="P4" s="3"/>
-      <c r="Q4" s="3"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4"/>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="4"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="E5" s="3" t="n">
+      <c r="E5" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="I5" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="J5" s="3" t="s">
+      <c r="J5" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="K5" s="3" t="s">
+      <c r="K5" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
-      <c r="O5" s="3"/>
-      <c r="P5" s="3"/>
-      <c r="Q5" s="3"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="4"/>
+      <c r="Q5" s="4"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="E6" s="3" t="n">
+      <c r="E6" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="G6" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="H6" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="I6" s="3" t="s">
+      <c r="I6" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="J6" s="3" t="s">
+      <c r="J6" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="K6" s="3" t="s">
+      <c r="K6" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
-      <c r="N6" s="3"/>
-      <c r="O6" s="3"/>
-      <c r="P6" s="3"/>
-      <c r="Q6" s="3"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4"/>
+      <c r="O6" s="4"/>
+      <c r="P6" s="4"/>
+      <c r="Q6" s="4"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="E7" s="3" t="n">
+      <c r="E7" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="G7" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="H7" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="I7" s="3" t="s">
+      <c r="I7" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="J7" s="3" t="s">
+      <c r="J7" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="K7" s="3" t="s">
+      <c r="K7" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
-      <c r="N7" s="3"/>
-      <c r="O7" s="3"/>
-      <c r="P7" s="3"/>
-      <c r="Q7" s="3"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="4"/>
+      <c r="O7" s="4"/>
+      <c r="P7" s="4"/>
+      <c r="Q7" s="4"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E8" s="3" t="n">
+      <c r="E8" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="G8" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="H8" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="I8" s="3" t="s">
+      <c r="I8" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="J8" s="3" t="s">
+      <c r="J8" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="K8" s="3" t="s">
+      <c r="K8" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
-      <c r="N8" s="3"/>
-      <c r="O8" s="3"/>
-      <c r="P8" s="3"/>
-      <c r="Q8" s="3"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="4"/>
+      <c r="P8" s="4"/>
+      <c r="Q8" s="4"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="E9" s="3" t="n">
+      <c r="E9" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="G9" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="H9" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="I9" s="3" t="s">
+      <c r="I9" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="J9" s="3" t="s">
+      <c r="J9" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="K9" s="3" t="s">
+      <c r="K9" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="L9" s="3"/>
-      <c r="M9" s="3"/>
-      <c r="N9" s="3"/>
-      <c r="O9" s="3"/>
-      <c r="P9" s="3"/>
-      <c r="Q9" s="3"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4"/>
+      <c r="O9" s="4"/>
+      <c r="P9" s="4"/>
+      <c r="Q9" s="4"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="E10" s="3" t="n">
+      <c r="E10" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="G10" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="H10" s="3" t="s">
+      <c r="H10" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="I10" s="3" t="s">
+      <c r="I10" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="J10" s="3" t="s">
+      <c r="J10" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="K10" s="3" t="s">
+      <c r="K10" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="L10" s="3"/>
-      <c r="M10" s="3"/>
-      <c r="N10" s="3"/>
-      <c r="O10" s="3"/>
-      <c r="P10" s="3"/>
-      <c r="Q10" s="3"/>
-    </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
+      <c r="N10" s="4"/>
+      <c r="O10" s="4"/>
+      <c r="P10" s="4"/>
+      <c r="Q10" s="4"/>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>